<commit_message>
Pay and Close doesn't close out order
</commit_message>
<xml_diff>
--- a/177c-restaurant/177c-table-design.xlsx
+++ b/177c-restaurant/177c-table-design.xlsx
@@ -105,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +115,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -139,6 +145,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +450,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +552,7 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="b">
+      <c r="C9" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -717,7 +724,7 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29" t="b">
+      <c r="F29" s="5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>